<commit_message>
fix: mapping name on excel table
</commit_message>
<xml_diff>
--- a/export_excel/transaction_9c5bb947-80ef-4204-8c79-7960205cdb84.xlsx
+++ b/export_excel/transaction_9c5bb947-80ef-4204-8c79-7960205cdb84.xlsx
@@ -19,13 +19,13 @@
     <t>Transaction ID</t>
   </si>
   <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Total Amount</t>
   </si>
   <si>
     <t>9c5bb947-80ef-4204-8c79-7960205cdb84</t>

</xml_diff>